<commit_message>
adding input files to skelton code
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/Banking Data/DataElements.xlsx
+++ b/SoftwareDesignUsingNLP/data/Banking Data/DataElements.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Dataelements" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Bill_type</t>
   </si>
   <si>
-    <t>This specifies the type of bills that will be withdrawn from ATM</t>
-  </si>
-  <si>
     <t>Max_limit</t>
   </si>
   <si>
@@ -150,18 +147,12 @@
     <t>Loan_purp</t>
   </si>
   <si>
-    <t>This signifies the purpose of taking loan like cbuying new car or house</t>
-  </si>
-  <si>
     <t>How much loan amount customer is asking. For applying loan this is must have</t>
   </si>
   <si>
     <t>Cred_Score</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer Name  and will be used for verification, deposit , withdrawal, transfer of money and for all activities </t>
-  </si>
-  <si>
     <t>Account Type will specify which type of account it is and will be used for deposit,  withddrawl, etc</t>
   </si>
   <si>
@@ -171,7 +162,25 @@
     <t>For approving loan one has to perform credit check score which is obtained from external agencies</t>
   </si>
   <si>
-    <t>Account number of the customer will be used to deposit,withdrawal, verififcation, and other banking activities. It is used to review transactions</t>
+    <t>This signifies the purpose of apply loan like cbuying new car or house</t>
+  </si>
+  <si>
+    <t>DE17</t>
+  </si>
+  <si>
+    <t>Bill_amt</t>
+  </si>
+  <si>
+    <t>This is used to specify bill amount</t>
+  </si>
+  <si>
+    <t>This utility specifies the type of bills that needed for bill payment process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account number of the customer will be used to deposit cheque, get cheque book, deposit money, withdrawal, review transactions, verififcation, and other banking activities. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Name  and will be used for verification, deposit , deposit cheque, get cheque, withdraw cheque, withdraw money, transfer money, review transactions and for all activities </t>
   </si>
 </sst>
 </file>
@@ -616,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -646,7 +655,7 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -657,7 +666,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,7 +677,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -723,7 +732,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,7 +743,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,10 +751,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,10 +762,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -764,10 +773,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,10 +784,10 @@
         <v>16</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -786,10 +795,10 @@
         <v>17</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -797,10 +806,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,15 +817,22 @@
         <v>19</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>

</xml_diff>